<commit_message>
Modification des scripts deploiments
</commit_message>
<xml_diff>
--- a/deploy_app/SecurityGroups.xlsx
+++ b/deploy_app/SecurityGroups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\Git_Repo\SyncSecurityGroup\deploy_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0456E09-8FE2-4B39-8669-65853BFF466D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C17466C-84BF-4543-B172-A5336B673F39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{A0467F55-60B7-4D52-87DC-63C5E24CD7B6}"/>
   </bookViews>
@@ -48,10 +48,10 @@
     <t>Second Security Group</t>
   </si>
   <si>
-    <t>941defb7-5620-43c1-80c9-4a5ea2846989</t>
-  </si>
-  <si>
-    <t>d93a3127-72fa-47d1-b774-0e867fa54dc7</t>
+    <t>4e37b55e-4df0-48d4-aefe-75d9d05ed21c</t>
+  </si>
+  <si>
+    <t>643a506c-55fd-460a-b8aa-6ac6c470b8ea</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -439,7 +439,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>